<commit_message>
Various fixes and updates to poll files.
- Include UAP figure for Essential and update files
related to that
- Fix sum-to-zero house effect constraint applying
to some parties it shouldn't and made changes to
make this less likely in future
- Add an old Nielsen poll to 2006vic
- Update preference flows for 2022fed.
Special note: for now UAP preference flows are
being given as the average of 2013/2019
elections. This is because while the 2019 UAP
campaigned along specifically anti-ALP lines,
2013 PUP was more generally anti-majors and
the present campaign is more in line with that,
so using last-election preferences may
underestimate the ALP's preference flow
somewhat.
</commit_message>
<xml_diff>
--- a/Preference Flow.xlsx
+++ b/Preference Flow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCEE12C-E665-44CA-A16F-8D5FA139523E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0278C9-74A9-41C4-A663-1D7D0FE43D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="11730" windowWidth="20280" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7140" yWindow="3795" windowWidth="29145" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
         <v>49.25</v>
       </c>
       <c r="J6">
-        <f>B6-B7</f>
+        <f t="shared" ref="J6:J12" si="1">B6-B7</f>
         <v>-1.0900000000000034</v>
       </c>
       <c r="K6">
@@ -632,11 +632,11 @@
         <v>5.43</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6:N12" si="1">F6-F7</f>
+        <f t="shared" ref="N6:N12" si="2">F6-F7</f>
         <v>2.5628985507246398</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O12" si="2">G6-G7</f>
+        <f t="shared" ref="O6:O12" si="3">G6-G7</f>
         <v>2.2800000000000011</v>
       </c>
     </row>
@@ -658,15 +658,15 @@
         <v>46.97</v>
       </c>
       <c r="J7">
-        <f>B7-B8</f>
+        <f t="shared" si="1"/>
         <v>4.1899999999999977</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9471014492753582</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.2299999999999969</v>
       </c>
     </row>
@@ -684,15 +684,15 @@
         <v>41.74</v>
       </c>
       <c r="J8">
-        <f>B8-B9</f>
+        <f t="shared" si="1"/>
         <v>-0.84999999999999432</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.8900000000000006</v>
       </c>
       <c r="O8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.8900000000000006</v>
       </c>
     </row>
@@ -710,15 +710,15 @@
         <v>44.63</v>
       </c>
       <c r="J9">
-        <f>B9-B10</f>
+        <f t="shared" si="1"/>
         <v>-1.1099999999999994</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.42999999999999972</v>
       </c>
       <c r="O9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.42999999999999972</v>
       </c>
     </row>
@@ -736,15 +736,15 @@
         <v>44.2</v>
       </c>
       <c r="J10">
-        <f>B10-B11</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-11.593877551020398</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.3999999999999986</v>
       </c>
     </row>
@@ -769,7 +769,7 @@
         <v>45.6</v>
       </c>
       <c r="J11">
-        <f>B11-B12</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K11">
@@ -781,11 +781,11 @@
         <v>7.3999999999999915</v>
       </c>
       <c r="N11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.49387755102041098</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-8</v>
       </c>
     </row>
@@ -810,7 +810,7 @@
         <v>53.6</v>
       </c>
       <c r="J12">
-        <f>B12-B13</f>
+        <f t="shared" si="1"/>
         <v>6.2000000000000028</v>
       </c>
       <c r="M12">
@@ -818,11 +818,11 @@
         <v>2.7000000000000028</v>
       </c>
       <c r="N12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9801801801801702</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.1000000000000014</v>
       </c>
     </row>
@@ -883,8 +883,8 @@
       </c>
       <c r="N15" s="1"/>
       <c r="O15">
-        <f>SQRT(SUMSQ(B22:K25)/COUNT(B22:K25))</f>
-        <v>7.7724780356598506</v>
+        <f>SQRT(SUMSQ(B22:K25,K5:L12)/COUNT(B22:K25,K5:L12))</f>
+        <v>8.0569865494528727</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -923,8 +923,8 @@
       </c>
       <c r="N16" s="1"/>
       <c r="O16">
-        <f>COUNT(B22:K25)</f>
-        <v>27</v>
+        <f>COUNT(B22:K25,K5:L12)</f>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1037,8 +1037,8 @@
       </c>
       <c r="N19" s="1"/>
       <c r="O19">
-        <f>SQRT(SUMSQ(B23:K25)/COUNT(B23:K25))</f>
-        <v>6.2907754335658455</v>
+        <f>SQRT(SUMSQ(B23:K25,K6:L12)/COUNT(B23:K25,K6:L12))</f>
+        <v>6.1100503271249735</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1047,8 +1047,8 @@
       </c>
       <c r="N20" s="1"/>
       <c r="O20">
-        <f>COUNT(B23:K25)</f>
-        <v>18</v>
+        <f>COUNT(B23:K25,K6:L12)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1091,39 +1091,39 @@
         <v>2019</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:K24" si="3">C16-C17</f>
+        <f t="shared" ref="C22:K24" si="4">C16-C17</f>
         <v>2.7800000000000011</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-13.96</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1.6799999999999997</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.68000000000000682</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.43</v>
       </c>
       <c r="H22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.0499999999999972</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-14.730000000000004</v>
       </c>
       <c r="J22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-19.34</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.09</v>
       </c>
     </row>
@@ -1136,39 +1136,39 @@
         <v>-1.3999999999999986</v>
       </c>
       <c r="C23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.48000000000000398</v>
       </c>
       <c r="D23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.96000000000000085</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1.2099999999999973</v>
       </c>
       <c r="F23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.8500000000000014</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.259999999999998</v>
       </c>
       <c r="H23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.759999999999998</v>
       </c>
       <c r="I23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.6300000000000026</v>
       </c>
       <c r="J23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.0799999999999983</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.4499999999999993</v>
       </c>
     </row>
@@ -1181,31 +1181,31 @@
         <v>1.490000000000002</v>
       </c>
       <c r="C24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.57</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9599999999999973</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5600000000000023</v>
       </c>
       <c r="H24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.5499999999999972</v>
       </c>
       <c r="I24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.31000000000000227</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.969999999999999</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.4899999999999984</v>
       </c>
     </row>

</xml_diff>